<commit_message>
1) Rotating mesh 2) Variable aoa for rotating mesh in change_bd.py 3) removing load from residuals.py
</commit_message>
<xml_diff>
--- a/OpenFoam/naca0012/naca0012.xlsx
+++ b/OpenFoam/naca0012/naca0012.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MarkDisk/Foam/DeepOpenFoam/OpenFoam/naca0012/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4725979-B073-5840-8E6F-61FC1B8535EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A222063D-F888-5C42-A078-772154708C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="37400" windowHeight="21100" xr2:uid="{58391FF8-9958-2343-AA59-3594AE5149CE}"/>
+    <workbookView xWindow="-21620" yWindow="-7160" windowWidth="21600" windowHeight="21100" xr2:uid="{58391FF8-9958-2343-AA59-3594AE5149CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -230,9 +230,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -243,6 +240,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2697,67 +2697,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>84667</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>61384</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="page8image49531328">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8CAECEA-DA8D-F048-8748-986E27CEEC93}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8509000" y="5312834"/>
-          <a:ext cx="3784600" cy="3395133"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -2788,7 +2727,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2821,7 +2760,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2851,6 +2790,50 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>340914</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>10584</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>767895</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>169334</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A002C08-8101-0F44-B56B-BB008E3947C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8595914" y="5238751"/>
+          <a:ext cx="4554481" cy="3577166"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -3157,21 +3140,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936A92A0-6A19-9844-B600-E9AFDED5A486}">
   <dimension ref="B1:M64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="H1" s="9">
+      <c r="H1" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9">
+      <c r="I1" s="13"/>
+      <c r="J1" s="13">
         <v>1.4E-3</v>
       </c>
-      <c r="K1" s="9"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
@@ -3849,16 +3832,16 @@
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="9"/>
+      <c r="C26" s="13"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3965,10 +3948,10 @@
       <c r="C46" s="14"/>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4035,10 +4018,10 @@
       <c r="C56" s="14"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C57" s="12" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Increasing the number of control points for the bezier case study: 12 point (10 dof)
</commit_message>
<xml_diff>
--- a/OpenFoam/naca0012/naca0012.xlsx
+++ b/OpenFoam/naca0012/naca0012.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MarkDisk/Foam/DeepOpenFoam/OpenFoam/naca0012/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A222063D-F888-5C42-A078-772154708C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C50976-CA9C-1344-A42F-88D3017F83E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21620" yWindow="-7160" windowWidth="21600" windowHeight="21100" xr2:uid="{58391FF8-9958-2343-AA59-3594AE5149CE}"/>
+    <workbookView xWindow="-21600" yWindow="-7160" windowWidth="21600" windowHeight="21100" xr2:uid="{58391FF8-9958-2343-AA59-3594AE5149CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Angle (deg)</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Spalart</t>
+  </si>
+  <si>
+    <t>Cl / Cd</t>
   </si>
 </sst>
 </file>
@@ -3138,15 +3141,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936A92A0-6A19-9844-B600-E9AFDED5A486}">
-  <dimension ref="B1:M64"/>
+  <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.2">
       <c r="H1" s="13">
         <v>0.14000000000000001</v>
       </c>
@@ -3155,8 +3158,9 @@
         <v>1.4E-3</v>
       </c>
       <c r="K1" s="13"/>
-    </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L1" s="13"/>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3187,11 +3191,14 @@
       <c r="K2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="L2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>0</v>
       </c>
@@ -3208,11 +3215,11 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F23" si="0">$M$3*D3</f>
+        <f>$O$3*D3</f>
         <v>45</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G23" si="1">$M$3*E3</f>
+        <f>$O$3*E3</f>
         <v>0</v>
       </c>
       <c r="H3" s="1">
@@ -3227,57 +3234,61 @@
       <c r="K3">
         <v>9.832604E-3</v>
       </c>
-      <c r="M3">
+      <c r="L3">
+        <f>J3/K3</f>
+        <v>1.4505496204260846E-2</v>
+      </c>
+      <c r="O3">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C23" si="2">PI()*B4/180</f>
+        <f t="shared" ref="C4:C23" si="0">PI()*B4/180</f>
         <v>1.7453292519943295E-2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D18" si="3">COS(C4)</f>
+        <f t="shared" ref="D4:D18" si="1">COS(C4)</f>
         <v>0.99984769515639127</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E23" si="4">SIN(C4)</f>
+        <f t="shared" ref="E4:E23" si="2">SIN(C4)</f>
         <v>1.7452406437283512E-2</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f>$O$3*D4</f>
         <v>44.993146282037607</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f>$O$3*E4</f>
         <v>0.785358289677758</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4906585039886591E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99939082701909576</v>
+      </c>
+      <c r="E5" s="2">
         <f t="shared" si="2"/>
-        <v>3.4906585039886591E-2</v>
-      </c>
-      <c r="D5" s="2">
-        <f t="shared" si="3"/>
-        <v>0.99939082701909576</v>
-      </c>
-      <c r="E5" s="2">
-        <f t="shared" si="4"/>
         <v>3.4899496702500969E-2</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="0"/>
+        <f>$O$3*D5</f>
         <v>44.972587215859306</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="1"/>
+        <f>$O$3*E5</f>
         <v>1.5704773516125436</v>
       </c>
       <c r="H5" s="4">
@@ -3292,54 +3303,58 @@
       <c r="K5">
         <v>1.0105299999999999E-2</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <f t="shared" ref="L4:L23" si="3">J5/K5</f>
+        <v>21.468645166397831</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>0.99862953475457383</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="2"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="3"/>
-        <v>0.99862953475457383</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="4"/>
         <v>5.2335956242943828E-2</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f>$O$3*D6</f>
         <v>44.93832906395582</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f>$O$3*E6</f>
         <v>2.3551180309324722</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>4</v>
       </c>
       <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>6.9813170079773182E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.9975640502598242</v>
+      </c>
+      <c r="E7" s="2">
         <f t="shared" si="2"/>
-        <v>6.9813170079773182E-2</v>
-      </c>
-      <c r="D7" s="2">
-        <f t="shared" si="3"/>
-        <v>0.9975640502598242</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="4"/>
         <v>6.9756473744125302E-2</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="0"/>
+        <f>$O$3*D7</f>
         <v>44.890382261692089</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="1"/>
+        <f>$O$3*E7</f>
         <v>3.1390413184856385</v>
       </c>
       <c r="H7" s="5">
@@ -3354,54 +3369,58 @@
       <c r="K7">
         <v>1.09354E-2</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>39.519368290140278</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8">
+        <f t="shared" si="0"/>
+        <v>8.7266462599716474E-2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0.99619469809174555</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="2"/>
-        <v>8.7266462599716474E-2</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="3"/>
-        <v>0.99619469809174555</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="4"/>
         <v>8.7155742747658166E-2</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f>$O$3*D8</f>
         <v>44.82876141412855</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f>$O$3*E8</f>
         <v>3.9220084236446175</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>6</v>
       </c>
       <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10471975511965977</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99452189536827329</v>
+      </c>
+      <c r="E9" s="2">
         <f t="shared" si="2"/>
-        <v>0.10471975511965977</v>
-      </c>
-      <c r="D9" s="2">
-        <f t="shared" si="3"/>
-        <v>0.99452189536827329</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" si="4"/>
         <v>0.10452846326765346</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="0"/>
+        <f>$O$3*D9</f>
         <v>44.753485291572296</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="1"/>
+        <f>$O$3*E9</f>
         <v>4.7037808470444054</v>
       </c>
       <c r="H9" s="4">
@@ -3416,54 +3435,58 @@
       <c r="K9">
         <v>1.238832E-2</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>51.984926123961927</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>7</v>
       </c>
       <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.12217304763960307</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>0.99254615164132198</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="2"/>
-        <v>0.12217304763960307</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="3"/>
-        <v>0.99254615164132198</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="4"/>
         <v>0.12186934340514748</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f>$O$3*D10</f>
         <v>44.664576823859491</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f>$O$3*E10</f>
         <v>5.4841204532316361</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>8</v>
       </c>
       <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13962634015954636</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99026806874157036</v>
+      </c>
+      <c r="E11" s="2">
         <f t="shared" si="2"/>
-        <v>0.13962634015954636</v>
-      </c>
-      <c r="D11" s="2">
-        <f t="shared" si="3"/>
-        <v>0.99026806874157036</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" si="4"/>
         <v>0.13917310096006544</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="0"/>
+        <f>$O$3*D11</f>
         <v>44.562063093370668</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="1"/>
+        <f>$O$3*E11</f>
         <v>6.2627895432029446</v>
       </c>
       <c r="H11" s="4">
@@ -3478,54 +3501,58 @@
       <c r="K11">
         <v>1.455306E-2</v>
       </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>58.427966352093655</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>9</v>
       </c>
       <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.15707963267948966</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>0.98768834059513777</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="2"/>
-        <v>0.15707963267948966</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="3"/>
-        <v>0.98768834059513777</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="4"/>
         <v>0.15643446504023087</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f>$O$3*D12</f>
         <v>44.445975326781202</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f>$O$3*E12</f>
         <v>7.0395509268103895</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>10</v>
       </c>
       <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.17453292519943295</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.98480775301220802</v>
+      </c>
+      <c r="E13" s="3">
         <f t="shared" si="2"/>
-        <v>0.17453292519943295</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="3"/>
-        <v>0.98480775301220802</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" si="4"/>
         <v>0.17364817766693033</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="0"/>
+        <f>$O$3*D13</f>
         <v>44.31634888554936</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="1"/>
+        <f>$O$3*E13</f>
         <v>7.8141679950118652</v>
       </c>
       <c r="H13" s="1">
@@ -3540,54 +3567,58 @@
       <c r="K13">
         <v>1.762292E-2</v>
       </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>59.43424812687114</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>11</v>
       </c>
       <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.19198621771937624</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>0.98162718344766398</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="2"/>
-        <v>0.19198621771937624</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="3"/>
-        <v>0.98162718344766398</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="4"/>
         <v>0.1908089953765448</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f>$O$3*D14</f>
         <v>44.173223255144876</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f>$O$3*E14</f>
         <v>8.586404791944517</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>12</v>
       </c>
       <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.20943951023931953</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>0.97814760073380569</v>
+      </c>
+      <c r="E15">
         <f t="shared" si="2"/>
-        <v>0.20943951023931953</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="3"/>
-        <v>0.97814760073380569</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="4"/>
         <v>0.20791169081775931</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f>$O$3*D15</f>
         <v>44.016642033021256</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f>$O$3*E15</f>
         <v>9.3560260867991687</v>
       </c>
       <c r="H15" s="1">
@@ -3602,54 +3633,58 @@
       <c r="K15">
         <v>2.196538E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>56.028031383932351</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>13</v>
       </c>
       <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.22689280275926285</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>0.97437006478523525</v>
+      </c>
+      <c r="E16">
         <f t="shared" si="2"/>
-        <v>0.22689280275926285</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="3"/>
-        <v>0.97437006478523525</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="4"/>
         <v>0.224951054343865</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f>$O$3*D16</f>
         <v>43.846652915335589</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f>$O$3*E16</f>
         <v>10.122797445473925</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>14</v>
       </c>
       <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.24434609527920614</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>0.97029572627599647</v>
+      </c>
+      <c r="E17">
         <f t="shared" si="2"/>
-        <v>0.24434609527920614</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="3"/>
-        <v>0.97029572627599647</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="4"/>
         <v>0.24192189559966773</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f>$O$3*D17</f>
         <v>43.663307682419841</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f>$O$3*E17</f>
         <v>10.886485301985047</v>
       </c>
       <c r="H17" s="1">
@@ -3664,50 +3699,54 @@
       <c r="K17">
         <v>2.8394679999999999E-2</v>
       </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>48.89813866541197</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>15</v>
       </c>
       <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.26179938779914941</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>0.96592582628906831</v>
+      </c>
+      <c r="E18">
         <f t="shared" si="2"/>
-        <v>0.26179938779914941</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="3"/>
-        <v>0.96592582628906831</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="4"/>
         <v>0.25881904510252074</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f>$O$3*D18</f>
         <v>43.466662183008076</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f>$O$3*E18</f>
         <v>11.646857029613432</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>16</v>
       </c>
       <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.27925268031909273</v>
+      </c>
+      <c r="E19">
         <f t="shared" si="2"/>
-        <v>0.27925268031909273</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="4"/>
         <v>0.27563735581699916</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f>$O$3*D19</f>
         <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f>$O$3*E19</f>
         <v>12.403681011764963</v>
       </c>
       <c r="H19" s="1">
@@ -3722,46 +3761,50 @@
       <c r="K19">
         <v>3.9604210000000001E-2</v>
       </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <f t="shared" si="3"/>
+        <v>37.761844005978148</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>17</v>
       </c>
       <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.29670597283903605</v>
+      </c>
+      <c r="E20">
         <f t="shared" si="2"/>
-        <v>0.29670597283903605</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="4"/>
         <v>0.29237170472273677</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f>$O$3*D20</f>
         <v>0</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f>$O$3*E20</f>
         <v>13.156726712523154</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>18</v>
       </c>
       <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0.31415926535897931</v>
+      </c>
+      <c r="E21">
         <f t="shared" si="2"/>
-        <v>0.31415926535897931</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="4"/>
         <v>0.3090169943749474</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f>$O$3*D21</f>
         <v>0</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f>$O$3*E21</f>
         <v>13.905764746872633</v>
       </c>
       <c r="H21" s="1">
@@ -3776,46 +3819,50 @@
       <c r="K21">
         <v>8.4611930000000002E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <f t="shared" si="3"/>
+        <v>15.871485262184658</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>19</v>
       </c>
       <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0.33161255787892258</v>
+      </c>
+      <c r="E22">
         <f t="shared" si="2"/>
-        <v>0.33161255787892258</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="4"/>
         <v>0.32556815445715664</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f>$O$3*D22</f>
         <v>0</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
+        <f>$O$3*E22</f>
         <v>14.650566950572049</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>20</v>
       </c>
       <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.3490658503988659</v>
+      </c>
+      <c r="E23">
         <f t="shared" si="2"/>
-        <v>0.3490658503988659</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="4"/>
         <v>0.34202014332566871</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f>$O$3*D23</f>
         <v>0</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
+        <f>$O$3*E23</f>
         <v>15.390906449655093</v>
       </c>
       <c r="H23" s="1">
@@ -3830,14 +3877,18 @@
       <c r="K23">
         <v>0.2270983</v>
       </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <f t="shared" si="3"/>
+        <v>3.8586387480663658</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="13"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27" s="9" t="s">
         <v>0</v>
       </c>
@@ -3845,7 +3896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>-4.59286799746223E-2</v>
       </c>
@@ -3853,7 +3904,7 @@
         <v>-4.9572876554684299E-3</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>3.02106847253574</v>
       </c>
@@ -3861,7 +3912,7 @@
         <v>0.30739314536950901</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>4.9890231487628798</v>
       </c>
@@ -3869,7 +3920,7 @@
         <v>0.52055651455465501</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>6.7729385207807704</v>
       </c>
@@ -3877,7 +3928,7 @@
         <v>0.74357249295504402</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>8.9249325012171905</v>
       </c>
@@ -4084,10 +4135,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B56:C56"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>